<commit_message>
feat: added new Input
</commit_message>
<xml_diff>
--- a/assets/worksheet.xlsx
+++ b/assets/worksheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="815">
   <si>
     <t xml:space="preserve">Stock_Central</t>
   </si>
@@ -2462,6 +2462,9 @@
   </si>
   <si>
     <t xml:space="preserve">Savon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooking Pots</t>
   </si>
 </sst>
 </file>
@@ -2471,7 +2474,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2532,6 +2535,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2575,7 +2585,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2605,6 +2615,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2799,8 +2813,8 @@
   </sheetPr>
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7212,7 +7226,9 @@
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
+      <c r="C66" s="8" t="s">
+        <v>814</v>
+      </c>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>

</xml_diff>